<commit_message>
añadimos cambios en los css
</commit_message>
<xml_diff>
--- a/faltas/src/faltas-de-material.xlsx
+++ b/faltas/src/faltas-de-material.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Número de Proyecto</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>repartidor</t>
+  </si>
+  <si>
+    <t>SE.M922606</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,7 +574,7 @@
         <v>20</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -616,6 +619,20 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>